<commit_message>
Update results; add shiny app code.
</commit_message>
<xml_diff>
--- a/data/CMIP5_models.xlsx
+++ b/data/CMIP5_models.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniepeacock/Salmon Watersheds Dropbox/Stephanie Peacock/X Drive/1_PROJECTS/1_Active/Climate Change/Data &amp; Analysis/Code/climate-change/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniepeacock/Salmon Watersheds Dropbox/Stephanie Peacock/X Drive/1_PROJECTS/1_Active/Climate Change/Data &amp; Analysis/ccva/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12477B0D-130E-414D-A488-2B810C5E6BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C910C0C-96D0-CE49-A962-865A91E137D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="1400" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{165DB4F0-2EBF-F04E-BFA8-F45732502208}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="97">
   <si>
     <t>Table 1</t>
   </si>
@@ -401,12 +401,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -427,9 +426,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -467,7 +466,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -573,7 +572,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -715,7 +714,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -772,7 +771,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>88</v>
       </c>
       <c r="B5" t="s">
@@ -789,7 +788,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1441,199 +1440,297 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002C1A39-1E05-B74A-B987-55F0205E9969}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D12"/>
+      <selection activeCell="C21" sqref="A15:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>